<commit_message>
improvements and test on GHFDB import
</commit_message>
<xml_diff>
--- a/tests/data/importer_success.xlsx
+++ b/tests/data/importer_success.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennings\Documents\repos\global-heat-flow-database\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C817E76-EE1D-4143-8A8C-3DCD644A7203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F58432-0852-4F31-869A-596D6CB9B3C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="1020" windowWidth="17080" windowHeight="6500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="427">
   <si>
     <t>M</t>
   </si>
@@ -1299,6 +1299,15 @@
   </si>
   <si>
     <t>sediment;granite</t>
+  </si>
+  <si>
+    <t>Continental</t>
+  </si>
+  <si>
+    <t>Southern Europe</t>
+  </si>
+  <si>
+    <t>Test Expedition</t>
   </si>
 </sst>
 </file>
@@ -2164,10 +2173,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BB1" sqref="BB1"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -2229,13 +2238,13 @@
     <col min="61" max="61" width="9.1796875" style="33"/>
     <col min="62" max="62" width="17" style="33" customWidth="1"/>
     <col min="63" max="63" width="9.1796875" style="33"/>
-    <col min="64" max="64" width="10.6328125" style="33" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="13.81640625" style="33" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="8.453125" style="33" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="7.26953125" style="33" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="8.453125" style="33" hidden="1" customWidth="1"/>
-    <col min="69" max="70" width="9.7265625" style="33" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="11.90625" style="33" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="10.6328125" style="33" customWidth="1"/>
+    <col min="65" max="65" width="13.81640625" style="33" customWidth="1"/>
+    <col min="66" max="66" width="8.453125" style="33" customWidth="1"/>
+    <col min="67" max="67" width="7.26953125" style="33" customWidth="1"/>
+    <col min="68" max="68" width="8.453125" style="33" customWidth="1"/>
+    <col min="69" max="70" width="9.7265625" style="33" customWidth="1"/>
+    <col min="71" max="71" width="11.90625" style="33" customWidth="1"/>
     <col min="72" max="72" width="4.1796875" style="75" customWidth="1"/>
     <col min="73" max="73" width="14.453125" style="78" customWidth="1"/>
     <col min="74" max="75" width="7.81640625" style="76" customWidth="1"/>
@@ -4094,7 +4103,9 @@
       <c r="S9" s="41">
         <v>45</v>
       </c>
-      <c r="T9" s="68"/>
+      <c r="T9" s="68">
+        <v>6.5</v>
+      </c>
       <c r="U9" s="40" t="s">
         <v>412</v>
       </c>
@@ -4106,7 +4117,7 @@
         <v>420</v>
       </c>
       <c r="Y9" s="44" t="s">
-        <v>233</v>
+        <v>347</v>
       </c>
       <c r="Z9" s="44" t="s">
         <v>233</v>
@@ -4132,8 +4143,12 @@
       <c r="AG9" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="AH9" s="44"/>
-      <c r="AI9" s="82"/>
+      <c r="AH9" s="44" t="s">
+        <v>426</v>
+      </c>
+      <c r="AI9" s="82" t="s">
+        <v>255</v>
+      </c>
       <c r="AJ9" s="49">
         <v>12</v>
       </c>
@@ -4226,11 +4241,15 @@
       <c r="BO9" s="43" t="s">
         <v>414</v>
       </c>
-      <c r="BP9" s="43"/>
+      <c r="BP9" s="43" t="s">
+        <v>425</v>
+      </c>
       <c r="BQ9" s="43" t="s">
         <v>416</v>
       </c>
-      <c r="BR9" s="43"/>
+      <c r="BR9" s="43" t="s">
+        <v>424</v>
+      </c>
       <c r="BS9" s="43"/>
       <c r="BT9" s="33"/>
       <c r="BU9" s="33"/>

</xml_diff>

<commit_message>
Merge from GFZ branch (#47)
* update docker-compose

* remove references to non-existent env files

* add domain to trusted origins

* add CSRF_TRUSTED_ORIGINS

* update docker compose

* add compress command to setup

* update fairdm

* updated fairdm

* minor_updates

* improvements and test on GHFDB import

* fairdm updates
</commit_message>
<xml_diff>
--- a/tests/data/importer_success.xlsx
+++ b/tests/data/importer_success.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennings\Documents\repos\global-heat-flow-database\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C817E76-EE1D-4143-8A8C-3DCD644A7203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F58432-0852-4F31-869A-596D6CB9B3C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="1020" windowWidth="17080" windowHeight="6500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="427">
   <si>
     <t>M</t>
   </si>
@@ -1299,6 +1299,15 @@
   </si>
   <si>
     <t>sediment;granite</t>
+  </si>
+  <si>
+    <t>Continental</t>
+  </si>
+  <si>
+    <t>Southern Europe</t>
+  </si>
+  <si>
+    <t>Test Expedition</t>
   </si>
 </sst>
 </file>
@@ -2164,10 +2173,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BB1" sqref="BB1"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -2229,13 +2238,13 @@
     <col min="61" max="61" width="9.1796875" style="33"/>
     <col min="62" max="62" width="17" style="33" customWidth="1"/>
     <col min="63" max="63" width="9.1796875" style="33"/>
-    <col min="64" max="64" width="10.6328125" style="33" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="13.81640625" style="33" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="8.453125" style="33" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="7.26953125" style="33" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="8.453125" style="33" hidden="1" customWidth="1"/>
-    <col min="69" max="70" width="9.7265625" style="33" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="11.90625" style="33" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="10.6328125" style="33" customWidth="1"/>
+    <col min="65" max="65" width="13.81640625" style="33" customWidth="1"/>
+    <col min="66" max="66" width="8.453125" style="33" customWidth="1"/>
+    <col min="67" max="67" width="7.26953125" style="33" customWidth="1"/>
+    <col min="68" max="68" width="8.453125" style="33" customWidth="1"/>
+    <col min="69" max="70" width="9.7265625" style="33" customWidth="1"/>
+    <col min="71" max="71" width="11.90625" style="33" customWidth="1"/>
     <col min="72" max="72" width="4.1796875" style="75" customWidth="1"/>
     <col min="73" max="73" width="14.453125" style="78" customWidth="1"/>
     <col min="74" max="75" width="7.81640625" style="76" customWidth="1"/>
@@ -4094,7 +4103,9 @@
       <c r="S9" s="41">
         <v>45</v>
       </c>
-      <c r="T9" s="68"/>
+      <c r="T9" s="68">
+        <v>6.5</v>
+      </c>
       <c r="U9" s="40" t="s">
         <v>412</v>
       </c>
@@ -4106,7 +4117,7 @@
         <v>420</v>
       </c>
       <c r="Y9" s="44" t="s">
-        <v>233</v>
+        <v>347</v>
       </c>
       <c r="Z9" s="44" t="s">
         <v>233</v>
@@ -4132,8 +4143,12 @@
       <c r="AG9" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="AH9" s="44"/>
-      <c r="AI9" s="82"/>
+      <c r="AH9" s="44" t="s">
+        <v>426</v>
+      </c>
+      <c r="AI9" s="82" t="s">
+        <v>255</v>
+      </c>
       <c r="AJ9" s="49">
         <v>12</v>
       </c>
@@ -4226,11 +4241,15 @@
       <c r="BO9" s="43" t="s">
         <v>414</v>
       </c>
-      <c r="BP9" s="43"/>
+      <c r="BP9" s="43" t="s">
+        <v>425</v>
+      </c>
       <c r="BQ9" s="43" t="s">
         <v>416</v>
       </c>
-      <c r="BR9" s="43"/>
+      <c r="BR9" s="43" t="s">
+        <v>424</v>
+      </c>
       <c r="BS9" s="43"/>
       <c r="BT9" s="33"/>
       <c r="BU9" s="33"/>

</xml_diff>